<commit_message>
NFP data preprocessing refactor
</commit_message>
<xml_diff>
--- a/raw/ijc_717.xlsx
+++ b/raw/ijc_717.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\blp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CF10404-473B-4433-8718-42B94C59B850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE14DECD-D9C9-4D27-B152-CC16F66F1AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="4395" windowWidth="28800" windowHeight="15345"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>INJCJC Index</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Actual</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>Prior</t>
   </si>
   <si>
@@ -70,13 +67,13 @@
     <t>Median Estimate</t>
   </si>
   <si>
-    <t>234k</t>
+    <t>233k</t>
   </si>
   <si>
     <t>Average Estimate</t>
   </si>
   <si>
-    <t>233.08k</t>
+    <t>233.01k</t>
   </si>
   <si>
     <t>High Estimate</t>
@@ -100,7 +97,7 @@
     <t>Standard Deviation</t>
   </si>
   <si>
-    <t>4.40k</t>
+    <t>4.37k</t>
   </si>
   <si>
     <t>Custom Estimate</t>
@@ -154,45 +151,45 @@
     <t>First Trust Portfolios LP</t>
   </si>
   <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>Michael Reid</t>
+  </si>
+  <si>
+    <t>RBC Capital Markets LLC</t>
+  </si>
+  <si>
+    <t>Derek Holt</t>
+  </si>
+  <si>
+    <t>Scotiabank</t>
+  </si>
+  <si>
+    <t>Crandall/Jordan</t>
+  </si>
+  <si>
+    <t>Wrightson ICAP LLC</t>
+  </si>
+  <si>
+    <t>Patrick Franke</t>
+  </si>
+  <si>
+    <t>Helaba Frankfurt</t>
+  </si>
+  <si>
+    <t>Standard Chartered PLC</t>
+  </si>
+  <si>
+    <t>Michael R Englund</t>
+  </si>
+  <si>
+    <t>Action Economics LLC</t>
+  </si>
+  <si>
     <t>5th</t>
   </si>
   <si>
-    <t>Michael Reid</t>
-  </si>
-  <si>
-    <t>RBC Capital Markets LLC</t>
-  </si>
-  <si>
-    <t>Derek Holt</t>
-  </si>
-  <si>
-    <t>Scotiabank</t>
-  </si>
-  <si>
-    <t>Crandall/Jordan</t>
-  </si>
-  <si>
-    <t>Wrightson ICAP LLC</t>
-  </si>
-  <si>
-    <t>Patrick Franke</t>
-  </si>
-  <si>
-    <t>Helaba Frankfurt</t>
-  </si>
-  <si>
-    <t>Standard Chartered PLC</t>
-  </si>
-  <si>
-    <t>Michael R Englund</t>
-  </si>
-  <si>
-    <t>Action Economics LLC</t>
-  </si>
-  <si>
-    <t>4th</t>
-  </si>
-  <si>
     <t>Rhys Herbert</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
     <t>JP Morgan Securities LLC</t>
   </si>
   <si>
+    <t>6th</t>
+  </si>
+  <si>
     <t>David P Kelly</t>
   </si>
   <si>
@@ -301,9 +301,6 @@
     <t>UBS Securities LLC</t>
   </si>
   <si>
-    <t>6th</t>
-  </si>
-  <si>
     <t>Nash Peyton</t>
   </si>
   <si>
@@ -365,6 +362,15 @@
   </si>
   <si>
     <t>Ameriprise Financial Inc</t>
+  </si>
+  <si>
+    <t>Marc Giannoni</t>
+  </si>
+  <si>
+    <t>Barclays Capital Inc.</t>
+  </si>
+  <si>
+    <t>7/16/2025</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1215,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R28" sqref="R28"/>
@@ -1299,8 +1305,8 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
+      <c r="C7" s="1">
+        <v>221</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1309,7 +1315,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>227</v>
@@ -1321,10 +1327,10 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>228</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1340,7 +1346,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1351,10 +1357,10 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1363,10 +1369,10 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1375,10 +1381,10 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1387,10 +1393,10 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1399,10 +1405,10 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1411,7 +1417,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
         <v>34</v>
@@ -1423,10 +1429,10 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1435,7 +1441,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1452,7 +1458,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1463,48 +1469,48 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1">
         <v>240</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D24" s="1">
         <v>232</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -1512,13 +1518,13 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="1">
         <v>228</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1526,111 +1532,111 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1">
         <v>240</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D27" s="1">
         <v>233</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D28" s="1">
         <v>232</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D29" s="1">
         <v>240</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D30" s="1">
         <v>235</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D31" s="1">
         <v>230</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D32" s="1">
         <v>235</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1638,63 +1644,63 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="1">
         <v>235</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D34" s="1">
         <v>237</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D35" s="1">
         <v>240</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D36" s="1">
         <v>232</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -1702,45 +1708,45 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="1">
         <v>230</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D38" s="1">
         <v>230</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D39" s="1">
         <v>234</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -1748,77 +1754,77 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="1">
         <v>232</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D41" s="1">
         <v>230</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D42" s="1">
         <v>220</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D43" s="1">
         <v>231</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D44" s="1">
         <v>232</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F44" s="1"/>
     </row>
@@ -1826,63 +1832,65 @@
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" s="1">
         <v>235</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D46" s="1">
         <v>231</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="1">
         <v>234</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D48" s="1">
         <v>230</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
@@ -1896,7 +1904,7 @@
         <v>234</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F49" s="1"/>
     </row>
@@ -1912,7 +1920,7 @@
         <v>235</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -1974,17 +1982,15 @@
       <c r="E54" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D55" s="1">
         <v>235</v>
@@ -1998,153 +2004,169 @@
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D56" s="1">
         <v>225</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D57" s="1">
         <v>235</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D58" s="1">
         <v>238</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D59" s="1">
         <v>239</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D60" s="1">
         <v>224</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D61" s="1">
         <v>240</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D62" s="1">
         <v>229</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D63" s="1">
         <v>231</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D64" s="1">
         <v>230</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="1">
+        <v>230</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>